<commit_message>
trying to make it work
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\VNTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3BAB2346-1FE7-47E6-B848-D00AEE045334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A708B56C-A37D-4798-823F-91BDF3FC40E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="decisions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -482,7 +482,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -612,6 +612,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -657,7 +694,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -687,6 +724,15 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1042,11 +1088,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E10" sqref="E10:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1095,7 +1141,7 @@
       <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -1117,9 +1163,7 @@
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="C3" s="13"/>
       <c r="D3" s="10" t="s">
         <v>8</v>
       </c>
@@ -1139,7 +1183,7 @@
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -1159,9 +1203,7 @@
       <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="C5" s="13"/>
       <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
@@ -1181,7 +1223,7 @@
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1205,9 +1247,7 @@
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="C7" s="13"/>
       <c r="D7" s="10" t="s">
         <v>12</v>
       </c>
@@ -1229,7 +1269,7 @@
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -1249,9 +1289,7 @@
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="C9" s="13"/>
       <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
@@ -1271,15 +1309,13 @@
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="8">
-        <v>5</v>
-      </c>
+      <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="10"/>
@@ -1293,15 +1329,11 @@
       <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="C11" s="14"/>
       <c r="D11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="8">
-        <v>5</v>
-      </c>
+      <c r="E11" s="8"/>
       <c r="F11" s="8">
         <v>2</v>
       </c>
@@ -1317,15 +1349,11 @@
       <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="C12" s="14"/>
       <c r="D12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="8">
-        <v>5</v>
-      </c>
+      <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <v>2</v>
@@ -1341,15 +1369,11 @@
       <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="C13" s="13"/>
       <c r="D13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="8">
-        <v>5</v>
-      </c>
+      <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="10"/>
@@ -1363,7 +1387,7 @@
       <c r="B14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -1385,9 +1409,7 @@
       <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="C15" s="13"/>
       <c r="D15" s="10" t="s">
         <v>22</v>
       </c>
@@ -1447,7 +1469,7 @@
       <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="10" t="s">
@@ -1469,9 +1491,7 @@
       <c r="B19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="C19" s="13"/>
       <c r="D19" s="10" t="s">
         <v>22</v>
       </c>
@@ -1531,6 +1551,15 @@
       <c r="J21" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
maybe, just maybe i will can use this power...
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\VNTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBC7CA7-F572-45F6-A845-3F7A108E1A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEF4EAC-44AC-4473-B65F-3A74ED7E0879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="decisions" sheetId="1" r:id="rId1"/>
+    <sheet name="decisions3" sheetId="2" r:id="rId1"/>
+    <sheet name="decisions" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -140,6 +141,15 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>Pasas la prueba final</t>
+  </si>
+  <si>
+    <t>NO pasas la prueba final</t>
+  </si>
+  <si>
+    <t>El jefe NO te interrumpe</t>
   </si>
 </sst>
 </file>
@@ -1094,11 +1104,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78677E5E-F13F-4F92-8D9F-E9DB85263F5F}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1558,8 +1568,486 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C13"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C18:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="14.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="2" customWidth="1"/>
+    <col min="8" max="10" width="11.42578125" style="4"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
+        <v>4</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
+        <v>2</v>
+      </c>
+      <c r="G6" s="8">
+        <v>-2</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8">
+        <v>-2</v>
+      </c>
+      <c r="G7" s="8">
+        <v>2</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8">
+        <v>2</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8">
+        <v>3</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="8">
+        <v>3</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="8">
+        <v>4</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
+        <v>3</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8">
+        <v>3</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8">
+        <v>3</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8">
+        <v>3</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C6:C7"/>

</xml_diff>